<commit_message>
v.2.0 Final (rendu E1)
</commit_message>
<xml_diff>
--- a/documentation/133-GestProjet-BOU-ANG.xlsx
+++ b/documentation/133-GestProjet-BOU-ANG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/noam_bourqui_studentfr_ch/Documents/Modules/3eme/133/projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D7E5D11-0013-49CB-92D3-F6DF0F3DD04E}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6A2CEC-94F3-4226-831D-32AEC0C4322B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
   <si>
     <t>Planning</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Schéma Séquence, Activité, Navigation &amp; Diagramme de classes</t>
-  </si>
-  <si>
-    <t>Diagramme de classes, documentation, gestion de projet</t>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
@@ -347,17 +344,118 @@
     <t>Angel Illan / 300231</t>
   </si>
   <si>
-    <t>Maquette, Documentation, diagramme activité et sequence</t>
-  </si>
-  <si>
-    <t>Diagramme de classes, documentation, gestion de projet, implémentation de l'api Rest1 avec DB &amp; gateway</t>
+    <t>25.03.2025 - PM</t>
+  </si>
+  <si>
+    <t>Diagrammes supplémentaires et documentation du projet</t>
+  </si>
+  <si>
+    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest1 avec DB &amp; gateway</t>
+  </si>
+  <si>
+    <t>Continuation de l'implémentation API Rest1 avec DB et finalisation du modèle ER</t>
+  </si>
+  <si>
+    <t>Implémentation de l'API et tests finaux</t>
+  </si>
+  <si>
+    <t>Tests de l'API et préparation à la présentation finale</t>
+  </si>
+  <si>
+    <t>Revue finale et débogage</t>
+  </si>
+  <si>
+    <t>Préparation de la documentation finale</t>
+  </si>
+  <si>
+    <t>Finalisation de la documentation et mise à jour des derniers éléments</t>
+  </si>
+  <si>
+    <t>Démo et présentation finale</t>
+  </si>
+  <si>
+    <t>Descriptif du projet, Use case client &amp; rest</t>
+  </si>
+  <si>
+    <t>Finalisation du planning, schéma Use Case et diagramme d'activité</t>
+  </si>
+  <si>
+    <t>Diagrammes supplémentaires et mise à jour du planning</t>
+  </si>
+  <si>
+    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest2 avec DB &amp; gateway</t>
+  </si>
+  <si>
+    <t>Création du frontend pour la partie admin</t>
+  </si>
+  <si>
+    <t>Déploiement de la partie du backend sur le serveur docker</t>
+  </si>
+  <si>
+    <t>Lien entre la partie frontend et backend</t>
+  </si>
+  <si>
+    <t>Correction de bug</t>
+  </si>
+  <si>
+    <t>Finalisation de la db sur docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation des maquettes admin et schéma </t>
+  </si>
+  <si>
+    <t>Problème rencontré</t>
+  </si>
+  <si>
+    <t>Nous avons rencontré une erreur de connexion à la base de données due à des identifiants incorrects, ainsi qu’un dysfonctionnement au niveau de la gestion de la session via HttpSession</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ce qui a été contrôlé</t>
+    </r>
+  </si>
+  <si>
+    <t>Suite de l'implémentation API Rest1 avec DB &amp; tests d'intégration</t>
+  </si>
+  <si>
+    <t>Pour insérér des données, j'ai eu des problèmes de nom entre mes json, mes modèles et ma db. J'ai également eu des problèmmes au niveau de la session</t>
+  </si>
+  <si>
+    <t>Continuation de l'implémentation API Rest2 &amp; API gateway avec DB et finalisation du modèle ER</t>
+  </si>
+  <si>
+    <t>Suite de l'implémentation API Rest2 &amp; API gateway avec DB &amp; tests unitaires</t>
+  </si>
+  <si>
+    <t>Frontend API1 &amp; API2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +546,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -510,7 +635,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -909,11 +1034,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -946,9 +1086,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1082,6 +1219,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,6 +1271,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1394,10 +1567,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1408,64 +1581,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="58"/>
       <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="58">
+      <c r="M3" s="57">
         <v>300231</v>
       </c>
-      <c r="N3" s="59"/>
+      <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="58"/>
       <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1475,34 +1648,34 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="55" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="55" t="s">
+      <c r="F7" s="55"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="55" t="s">
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="55" t="s">
+      <c r="L7" s="55"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="56"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="56"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1555,517 +1728,544 @@
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="29"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="29"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="28"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="29"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="28"/>
     </row>
     <row r="12" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="30" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="29"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="27" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="29"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="27" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="29"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="28"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="28"/>
     </row>
     <row r="16" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="30" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="28"/>
     </row>
     <row r="17" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="28"/>
     </row>
     <row r="18" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="31" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
     </row>
     <row r="20" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
     </row>
     <row r="21" spans="1:16" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
     </row>
     <row r="22" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="29"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
     </row>
     <row r="24" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="29"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="27"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
     </row>
     <row r="25" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K25" s="27"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="29"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
     </row>
     <row r="26" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" s="33"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="35"/>
+    </row>
+    <row r="27" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="36"/>
-    </row>
-    <row r="27" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="36"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="34"/>
+      <c r="P27" s="35"/>
     </row>
     <row r="28" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" s="34"/>
+      <c r="P28" s="35"/>
+    </row>
+    <row r="29" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="36"/>
-    </row>
-    <row r="29" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="34"/>
+      <c r="P29" s="35"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="36"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="29"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="28"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="43"/>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="44"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="51"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32" s="51"/>
+      <c r="N32" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="O32" s="53"/>
+      <c r="P32" s="51"/>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="54"/>
-      <c r="P32" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2093,46 +2293,49 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C12:C13"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="72"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C4" s="72"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>55</v>
       </c>
@@ -2142,141 +2345,221 @@
       <c r="C7" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>45740</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="D7" s="65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="61">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>45741</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="D8" s="61"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="61"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C10" s="61">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>45747</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="D10" s="61"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="61"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="61"/>
+    </row>
+    <row r="13" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="61"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="61"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="61"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D17" s="61"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D18" s="61"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D19" s="61"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="D20" s="61"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="C21" s="14">
+        <f>SUM(C8:C20)</f>
+        <v>45.5</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="15">
-        <f>SUM(C8:C21)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
-        <v>67</v>
-      </c>
+      <c r="C28" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2289,10 +2572,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,26 +2583,28 @@
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2328,143 +2613,223 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="64" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>45740</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="15">
+      <c r="D7" s="65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="66">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>45741</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="D8" s="67"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="66">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>45747</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="D9" s="67"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="67"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="67"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="67"/>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="67"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="67"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D17" s="67"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D18" s="67"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D19" s="67"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D20" s="67"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="66">
+        <v>3.5</v>
+      </c>
+      <c r="D21" s="67"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="B22" s="70"/>
+      <c r="C22" s="71">
+        <f>SUM(C8:C21)</f>
+        <v>45.5</v>
+      </c>
+      <c r="D22" s="67"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="15">
-        <f>SUM(C8:C21)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2472,7 +2837,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2490,6 +2855,62 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="35" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c91a1a7a62e987314df808fa39da4b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e3023738844047246cab05fc3830165" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -2943,62 +3364,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
   <ds:schemaRefs>
@@ -3008,6 +3373,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05539879-8A52-4B74-9FF2-F471F780BCE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3025,15 +3401,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v.2.1 Final (rendu E1)
</commit_message>
<xml_diff>
--- a/documentation/133-GestProjet-BOU-ANG.xlsx
+++ b/documentation/133-GestProjet-BOU-ANG.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28816"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/noam_bourqui_studentfr_ch/Documents/Modules/3eme/133/projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6A2CEC-94F3-4226-831D-32AEC0C4322B}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE735D2-9B76-404B-8678-8B7340516E87}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
-    <sheet name="Journal de travail BOU" sheetId="2" r:id="rId2"/>
-    <sheet name="Journal de travail ANG" sheetId="5" r:id="rId3"/>
+    <sheet name="Journal de travail ANG" sheetId="5" r:id="rId2"/>
+    <sheet name="Journal de travail BOU" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="97">
   <si>
     <t>Planning</t>
   </si>
@@ -175,6 +175,9 @@
     <t>API BOU &amp; API ANG</t>
   </si>
   <si>
+    <t>Frontend API1 &amp; API2</t>
+  </si>
+  <si>
     <t>Tests de l'application</t>
   </si>
   <si>
@@ -202,7 +205,7 @@
     <t>Elève / classe</t>
   </si>
   <si>
-    <t>Bourqui Noam / 300231</t>
+    <t>Angel Illan / 300231</t>
   </si>
   <si>
     <t>Date</t>
@@ -214,10 +217,52 @@
     <t>Temps d'exécution [heures]</t>
   </si>
   <si>
-    <t>Gestion du planning, documentation &amp; schéma Use Case</t>
+    <t>Problème rencontré</t>
+  </si>
+  <si>
+    <t>Descriptif du projet, Use case client &amp; rest</t>
+  </si>
+  <si>
+    <t>Finalisation du planning, schéma Use Case et diagramme d'activité</t>
   </si>
   <si>
     <t>Schéma Séquence, Activité, Navigation &amp; Diagramme de classes</t>
+  </si>
+  <si>
+    <t>25.03.2025 - PM</t>
+  </si>
+  <si>
+    <t>Diagrammes supplémentaires et mise à jour du planning</t>
+  </si>
+  <si>
+    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest1 avec DB &amp; gateway</t>
+  </si>
+  <si>
+    <t>Continuation de l'implémentation API Rest1 avec DB et finalisation du modèle ER</t>
+  </si>
+  <si>
+    <t>Nous avons rencontré une erreur de connexion à la base de données due à des identifiants incorrects, ainsi qu’un dysfonctionnement au niveau de la gestion de la session via HttpSession</t>
+  </si>
+  <si>
+    <t>Suite de l'implémentation API Rest1 avec DB &amp; tests d'intégration</t>
+  </si>
+  <si>
+    <t>Implémentation de l'API et tests finaux</t>
+  </si>
+  <si>
+    <t>Tests de l'API et préparation à la présentation finale</t>
+  </si>
+  <si>
+    <t>Revue finale et débogage</t>
+  </si>
+  <si>
+    <t>Préparation de la documentation finale</t>
+  </si>
+  <si>
+    <t>Finalisation de la documentation et mise à jour des derniers éléments</t>
+  </si>
+  <si>
+    <t>Démo et présentation finale</t>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
@@ -293,121 +338,6 @@
       </rPr>
       <t>Toutes les rencontres avec le professeur</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ce qui a été contrôlé</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ce qui a été décidé</t>
-    </r>
-  </si>
-  <si>
-    <t>Angel Illan / 300231</t>
-  </si>
-  <si>
-    <t>25.03.2025 - PM</t>
-  </si>
-  <si>
-    <t>Diagrammes supplémentaires et documentation du projet</t>
-  </si>
-  <si>
-    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest1 avec DB &amp; gateway</t>
-  </si>
-  <si>
-    <t>Continuation de l'implémentation API Rest1 avec DB et finalisation du modèle ER</t>
-  </si>
-  <si>
-    <t>Implémentation de l'API et tests finaux</t>
-  </si>
-  <si>
-    <t>Tests de l'API et préparation à la présentation finale</t>
-  </si>
-  <si>
-    <t>Revue finale et débogage</t>
-  </si>
-  <si>
-    <t>Préparation de la documentation finale</t>
-  </si>
-  <si>
-    <t>Finalisation de la documentation et mise à jour des derniers éléments</t>
-  </si>
-  <si>
-    <t>Démo et présentation finale</t>
-  </si>
-  <si>
-    <t>Descriptif du projet, Use case client &amp; rest</t>
-  </si>
-  <si>
-    <t>Finalisation du planning, schéma Use Case et diagramme d'activité</t>
-  </si>
-  <si>
-    <t>Diagrammes supplémentaires et mise à jour du planning</t>
-  </si>
-  <si>
-    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest2 avec DB &amp; gateway</t>
-  </si>
-  <si>
-    <t>Création du frontend pour la partie admin</t>
-  </si>
-  <si>
-    <t>Déploiement de la partie du backend sur le serveur docker</t>
-  </si>
-  <si>
-    <t>Lien entre la partie frontend et backend</t>
-  </si>
-  <si>
-    <t>Correction de bug</t>
-  </si>
-  <si>
-    <t>Finalisation de la db sur docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalisation des maquettes admin et schéma </t>
-  </si>
-  <si>
-    <t>Problème rencontré</t>
-  </si>
-  <si>
-    <t>Nous avons rencontré une erreur de connexion à la base de données due à des identifiants incorrects, ainsi qu’un dysfonctionnement au niveau de la gestion de la session via HttpSession</t>
   </si>
   <si>
     <r>
@@ -436,26 +366,99 @@
     </r>
   </si>
   <si>
-    <t>Suite de l'implémentation API Rest1 avec DB &amp; tests d'intégration</t>
-  </si>
-  <si>
-    <t>Pour insérér des données, j'ai eu des problèmes de nom entre mes json, mes modèles et ma db. J'ai également eu des problèmmes au niveau de la session</t>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ce qui a été décidé</t>
+    </r>
+  </si>
+  <si>
+    <t>Bourqui Noam / 300231</t>
+  </si>
+  <si>
+    <t>Gestion du planning, documentation &amp; schéma Use Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation des maquettes admin et schéma </t>
+  </si>
+  <si>
+    <t>Diagrammes supplémentaires et documentation du projet</t>
+  </si>
+  <si>
+    <t>Diagramme de classes, gestion de projet, début de l'implémentation API Rest2 avec DB &amp; gateway</t>
   </si>
   <si>
     <t>Continuation de l'implémentation API Rest2 &amp; API gateway avec DB et finalisation du modèle ER</t>
   </si>
   <si>
-    <t>Suite de l'implémentation API Rest2 &amp; API gateway avec DB &amp; tests unitaires</t>
-  </si>
-  <si>
-    <t>Frontend API1 &amp; API2</t>
+    <t>Pour insérér des données, j'ai eu des problèmes de nom entre mes json, mes modèles et ma db. J'ai également eu des problèmmes au niveau de la session. Mais j'ai pu résoudre ces problèmes.</t>
+  </si>
+  <si>
+    <t>Suite de l'implémentation API Rest2 &amp; API gateway avec DB &amp; tests</t>
+  </si>
+  <si>
+    <t>Création du frontend pour la partie admin</t>
+  </si>
+  <si>
+    <t>Lien entre la partie frontend et backend</t>
+  </si>
+  <si>
+    <t>Déploiement de la partie du backend sur le serveur docker</t>
+  </si>
+  <si>
+    <t>Correction de bug</t>
+  </si>
+  <si>
+    <t>Finalisation de la db sur docker</t>
+  </si>
+  <si>
+    <t>J'étais malade, donc j'ai dû la faire chez moi.</t>
+  </si>
+  <si>
+    <r>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ce qui a été contrôlé</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1053,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1198,27 +1201,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1250,7 +1232,27 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,10 +1273,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1569,76 +1567,76 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A6" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="11" width="8" customWidth="1"/>
     <col min="12" max="17" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:16" ht="31.5">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:16" ht="21.75" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="58"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="57">
+      <c r="M3" s="68">
         <v>300231</v>
       </c>
-      <c r="N3" s="58"/>
-    </row>
-    <row r="4" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N3" s="69"/>
+    </row>
+    <row r="4" spans="1:16" ht="21.75" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="58"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="69"/>
       <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1646,35 +1644,35 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="54" t="s">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1">
+      <c r="B7" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="54" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="54" t="s">
+      <c r="F7" s="66"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="54" t="s">
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="54" t="s">
+      <c r="L7" s="66"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="55"/>
-      <c r="P7" s="56"/>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="66"/>
+      <c r="P7" s="67"/>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="96" customHeight="1">
       <c r="A8" s="20" t="s">
         <v>12</v>
       </c>
@@ -1724,7 +1722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.45" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -1752,7 +1750,7 @@
       <c r="O9" s="27"/>
       <c r="P9" s="28"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="5"/>
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
@@ -1770,7 +1768,7 @@
       <c r="O10" s="27"/>
       <c r="P10" s="28"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
@@ -1790,7 +1788,7 @@
       <c r="O11" s="27"/>
       <c r="P11" s="28"/>
     </row>
-    <row r="12" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" outlineLevel="1">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
@@ -1812,7 +1810,7 @@
       <c r="O12" s="27"/>
       <c r="P12" s="28"/>
     </row>
-    <row r="13" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" outlineLevel="1">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
@@ -1834,7 +1832,7 @@
       <c r="O13" s="27"/>
       <c r="P13" s="28"/>
     </row>
-    <row r="14" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" outlineLevel="1">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -1856,7 +1854,7 @@
       <c r="O14" s="27"/>
       <c r="P14" s="28"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -1878,7 +1876,7 @@
       <c r="O15" s="27"/>
       <c r="P15" s="28"/>
     </row>
-    <row r="16" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" outlineLevel="1">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -1900,7 +1898,7 @@
       <c r="O16" s="27"/>
       <c r="P16" s="28"/>
     </row>
-    <row r="17" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" outlineLevel="1">
       <c r="A17" s="8" t="s">
         <v>36</v>
       </c>
@@ -1920,7 +1918,7 @@
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
     </row>
-    <row r="18" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" outlineLevel="1">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1942,7 +1940,7 @@
       <c r="O18" s="27"/>
       <c r="P18" s="28"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="25" t="s">
         <v>38</v>
       </c>
@@ -1964,7 +1962,7 @@
       <c r="O19" s="27"/>
       <c r="P19" s="28"/>
     </row>
-    <row r="20" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" outlineLevel="1">
       <c r="A20" s="25" t="s">
         <v>39</v>
       </c>
@@ -1986,7 +1984,7 @@
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
     </row>
-    <row r="21" spans="1:16" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="30" outlineLevel="1">
       <c r="A21" s="25" t="s">
         <v>40</v>
       </c>
@@ -2008,7 +2006,7 @@
       <c r="O21" s="27"/>
       <c r="P21" s="28"/>
     </row>
-    <row r="22" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" outlineLevel="1">
       <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
@@ -2028,7 +2026,7 @@
       <c r="O22" s="27"/>
       <c r="P22" s="28"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
@@ -2048,7 +2046,7 @@
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
     </row>
-    <row r="24" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" outlineLevel="1">
       <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
@@ -2074,7 +2072,7 @@
       <c r="O24" s="27"/>
       <c r="P24" s="28"/>
     </row>
-    <row r="25" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" outlineLevel="1">
       <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
@@ -2102,9 +2100,9 @@
       <c r="O25" s="27"/>
       <c r="P25" s="28"/>
     </row>
-    <row r="26" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" outlineLevel="1">
       <c r="A26" s="5" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="B26" s="33"/>
       <c r="C26" s="34"/>
@@ -2126,9 +2124,9 @@
       <c r="O26" s="34"/>
       <c r="P26" s="35"/>
     </row>
-    <row r="27" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" outlineLevel="1">
       <c r="A27" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="34"/>
@@ -2148,9 +2146,9 @@
       <c r="O27" s="34"/>
       <c r="P27" s="35"/>
     </row>
-    <row r="28" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" outlineLevel="1">
       <c r="A28" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="34"/>
@@ -2170,9 +2168,9 @@
       <c r="O28" s="34"/>
       <c r="P28" s="35"/>
     </row>
-    <row r="29" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" outlineLevel="1">
       <c r="A29" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="34"/>
@@ -2192,9 +2190,9 @@
       <c r="O29" s="34"/>
       <c r="P29" s="35"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="27"/>
@@ -2212,9 +2210,9 @@
       <c r="O30" s="27"/>
       <c r="P30" s="28"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="27"/>
@@ -2230,11 +2228,13 @@
       <c r="M31" s="28"/>
       <c r="N31" s="41"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="43"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P31" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" thickBot="1">
       <c r="A32" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="44"/>
       <c r="C32" s="45"/>
@@ -2259,12 +2259,14 @@
       <c r="N32" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="53"/>
+      <c r="O32" s="53" t="s">
+        <v>29</v>
+      </c>
       <c r="P32" s="51"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" thickBot="1">
       <c r="A33" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2289,285 +2291,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:D28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D8" s="61"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="61"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D10" s="61"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D11" s="61"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="61"/>
-    </row>
-    <row r="13" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D14" s="61"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D15" s="61"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D16" s="61"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D17" s="61"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D18" s="61"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D19" s="61"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="61">
-        <v>3.5</v>
-      </c>
-      <c r="D20" s="61"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="14">
-        <f>SUM(C8:C20)</f>
-        <v>45.5</v>
-      </c>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="16"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="16"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
-    <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C633685-DDE5-4CA1-AE40-7C2F7C7D3A1F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2578,7 +2301,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
@@ -2587,24 +2310,24 @@
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="31.5">
+      <c r="A1" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:4" ht="21.75" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="21.75" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2613,223 +2336,223 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="64" t="s">
+    <row r="7" spans="1:4" ht="25.5">
+      <c r="A7" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="B7" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="C7" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="66">
+      <c r="B8" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="59">
         <v>3.5</v>
       </c>
-      <c r="D8" s="67"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="66" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="66">
+      <c r="B9" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="59">
         <v>3.5</v>
       </c>
-      <c r="D9" s="67"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="66">
+      <c r="B10" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="59">
         <v>3.5</v>
       </c>
-      <c r="D10" s="67"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="59">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="60"/>
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="59">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="60"/>
+    </row>
+    <row r="13" spans="1:4" ht="60">
+      <c r="A13" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="59">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="66">
+      <c r="C14" s="59">
         <v>3.5</v>
       </c>
-      <c r="D11" s="67"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="66" t="s">
+      <c r="D14" s="60"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="59">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="60"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="66">
+      <c r="C17" s="59">
         <v>3.5</v>
       </c>
-      <c r="D12" s="67"/>
-    </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="66" t="s">
+      <c r="D17" s="60"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="66">
+      <c r="C18" s="59">
         <v>3.5</v>
       </c>
-      <c r="D13" s="68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="66">
+      <c r="D18" s="60"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="59">
         <v>3.5</v>
       </c>
-      <c r="D14" s="67"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="67"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="66" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="66">
+      <c r="D19" s="60"/>
+    </row>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="59">
         <v>3.5</v>
       </c>
-      <c r="D16" s="67"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="66" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="66">
+      <c r="D20" s="60"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="59">
         <v>3.5</v>
       </c>
-      <c r="D17" s="67"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="66">
-        <v>3.5</v>
-      </c>
-      <c r="D18" s="67"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="66" t="s">
+      <c r="D21" s="60"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="66">
-        <v>3.5</v>
-      </c>
-      <c r="D19" s="67"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="66">
-        <v>3.5</v>
-      </c>
-      <c r="D20" s="67"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="66" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="66">
-        <v>3.5</v>
-      </c>
-      <c r="D21" s="67"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="71">
+      <c r="B22" s="63"/>
+      <c r="C22" s="64">
         <f>SUM(C8:C21)</f>
         <v>45.5</v>
       </c>
-      <c r="D22" s="67"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="60"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="B24" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="B25" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="B26" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="B27" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="B29" s="17" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2838,6 +2561,287 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
+    <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5">
+      <c r="A1" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:4" ht="21.75" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="54"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="54"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="54"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="54"/>
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="54"/>
+    </row>
+    <row r="13" spans="1:4" ht="121.5">
+      <c r="A13" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="54"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="54"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="54"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D17" s="54"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D18" s="54"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D19" s="54"/>
+    </row>
+    <row r="20" spans="1:4" ht="30.75">
+      <c r="A20" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14">
+        <f>SUM(C8:C20)</f>
+        <v>45.5</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2855,62 +2859,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="35" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c91a1a7a62e987314df808fa39da4b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e3023738844047246cab05fc3830165" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -3364,41 +3312,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05539879-8A52-4B74-9FF2-F471F780BCE4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05539879-8A52-4B74-9FF2-F471F780BCE4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}"/>
 </file>
</xml_diff>